<commit_message>
Update code & add error analysis
</commit_message>
<xml_diff>
--- a/data-munge/output/latin.xlsx
+++ b/data-munge/output/latin.xlsx
@@ -18048,7 +18048,10 @@
     <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>

</xml_diff>